<commit_message>
Update thumbnails to include only five-year intervals
</commit_message>
<xml_diff>
--- a/output_data/charts/0500000US39041.xlsx
+++ b/output_data/charts/0500000US39041.xlsx
@@ -137,17 +137,7 @@
       <c:layout/>
     </c:title>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.14000000000000001"/>
-          <c:y val="0.13"/>
-          <c:w val="0.80000000000000004"/>
-          <c:h val="0.67000000000000004"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:ser>
@@ -185,101 +175,41 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$32</c:f>
+              <c:f>Sheet1!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>36708</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>37073</c:v>
+                  <c:v>38534</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>37438</c:v>
+                  <c:v>40360</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37803</c:v>
+                  <c:v>42186</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>38169</c:v>
+                  <c:v>44013</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>38534</c:v>
+                  <c:v>45839</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>38899</c:v>
+                  <c:v>47665</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>39264</c:v>
+                  <c:v>49491</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>39630</c:v>
+                  <c:v>51318</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>39995</c:v>
+                  <c:v>53144</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>40360</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>40725</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>41091</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>41456</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>41821</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>42186</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>42552</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>42917</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>43282</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>43647</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>44013</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>44378</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>44743</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>45108</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>45292</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>45839</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>47665</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>49491</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>51318</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>53144</c:v>
-                </c:pt>
-                <c:pt idx="30">
                   <c:v>54970</c:v>
                 </c:pt>
               </c:numCache>
@@ -287,84 +217,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$32</c:f>
+              <c:f>Sheet1!$B$2:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>111759</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>118646</c:v>
+                  <c:v>149153</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>126172</c:v>
+                  <c:v>175149</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>133842</c:v>
+                  <c:v>194358</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>141348</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>149153</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>156164</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>161796</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>166652</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>170676</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>175149</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>178759</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>181549</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>186000</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>190243</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>194358</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>198317</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>202171</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>206501</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>211062</c:v>
-                </c:pt>
-                <c:pt idx="20">
                   <c:v>215166</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>221282</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>226526</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>231636</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>234305</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -396,101 +266,41 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$32</c:f>
+              <c:f>Sheet1!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>36708</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>37073</c:v>
+                  <c:v>38534</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>37438</c:v>
+                  <c:v>40360</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37803</c:v>
+                  <c:v>42186</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>38169</c:v>
+                  <c:v>44013</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>38534</c:v>
+                  <c:v>45839</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>38899</c:v>
+                  <c:v>47665</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>39264</c:v>
+                  <c:v>49491</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>39630</c:v>
+                  <c:v>51318</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>39995</c:v>
+                  <c:v>53144</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>40360</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>40725</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>41091</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>41456</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>41821</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>42186</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>42552</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>42917</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>43282</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>43647</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>44013</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>44378</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>44743</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>45108</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>45292</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>45839</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>47665</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>49491</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>51318</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>53144</c:v>
-                </c:pt>
-                <c:pt idx="30">
                   <c:v>54970</c:v>
                 </c:pt>
               </c:numCache>
@@ -498,26 +308,26 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$32</c:f>
+              <c:f>Sheet1!$C$2:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
-                <c:pt idx="25">
+                <c:ptCount val="11"/>
+                <c:pt idx="5">
                   <c:v>248441</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="6">
                   <c:v>287218</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="7">
                   <c:v>329249</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="8">
                   <c:v>373888</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="9">
                   <c:v>420768</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="10">
                   <c:v>469644</c:v>
                 </c:pt>
               </c:numCache>
@@ -550,101 +360,41 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$32</c:f>
+              <c:f>Sheet1!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>36708</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>37073</c:v>
+                  <c:v>38534</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>37438</c:v>
+                  <c:v>40360</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37803</c:v>
+                  <c:v>42186</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>38169</c:v>
+                  <c:v>44013</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>38534</c:v>
+                  <c:v>45839</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>38899</c:v>
+                  <c:v>47665</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>39264</c:v>
+                  <c:v>49491</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>39630</c:v>
+                  <c:v>51318</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>39995</c:v>
+                  <c:v>53144</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>40360</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>40725</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>41091</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>41456</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>41821</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>42186</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>42552</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>42917</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>43282</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>43647</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>44013</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>44378</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>44743</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>45108</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>45292</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>45839</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>47665</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>49491</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>51318</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>53144</c:v>
-                </c:pt>
-                <c:pt idx="30">
                   <c:v>54970</c:v>
                 </c:pt>
               </c:numCache>
@@ -652,26 +402,26 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$32</c:f>
+              <c:f>Sheet1!$D$2:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
-                <c:pt idx="25">
+                <c:ptCount val="11"/>
+                <c:pt idx="5">
                   <c:v>238464</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="6">
                   <c:v>256467</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="7">
                   <c:v>271216</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="8">
                   <c:v>283357</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="9">
                   <c:v>293257</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="10">
                   <c:v>301161</c:v>
                 </c:pt>
               </c:numCache>
@@ -713,101 +463,41 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$32</c:f>
+              <c:f>Sheet1!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>36708</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>37073</c:v>
+                  <c:v>38534</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>37438</c:v>
+                  <c:v>40360</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37803</c:v>
+                  <c:v>42186</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>38169</c:v>
+                  <c:v>44013</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>38534</c:v>
+                  <c:v>45839</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>38899</c:v>
+                  <c:v>47665</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>39264</c:v>
+                  <c:v>49491</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>39630</c:v>
+                  <c:v>51318</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>39995</c:v>
+                  <c:v>53144</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>40360</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>40725</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>41091</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>41456</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>41821</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>42186</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>42552</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>42917</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>43282</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>43647</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>44013</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>44378</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>44743</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>45108</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>45292</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>45839</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>47665</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>49491</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>51318</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>53144</c:v>
-                </c:pt>
-                <c:pt idx="30">
                   <c:v>54970</c:v>
                 </c:pt>
               </c:numCache>
@@ -815,26 +505,26 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$32</c:f>
+              <c:f>Sheet1!$E$2:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
-                <c:pt idx="25">
+                <c:ptCount val="11"/>
+                <c:pt idx="5">
                   <c:v>247016</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="6">
                   <c:v>277484</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="7">
                   <c:v>310863</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="8">
                   <c:v>340917</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="9">
                   <c:v>369307</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="10">
                   <c:v>397697</c:v>
                 </c:pt>
               </c:numCache>
@@ -849,6 +539,8 @@
         <c:axId val="50010001"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="54970.0"/>
+          <c:min val="36708.0"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy" sourceLinked="0"/>
@@ -1246,7 +938,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1286,277 +978,117 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="4">
-        <v>37073</v>
+        <v>38534</v>
       </c>
       <c r="B3" s="2">
-        <v>118646</v>
+        <v>149153</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="4">
-        <v>37438</v>
+        <v>40360</v>
       </c>
       <c r="B4" s="2">
-        <v>126172</v>
+        <v>175149</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="4">
-        <v>37803</v>
+        <v>42186</v>
       </c>
       <c r="B5" s="2">
-        <v>133842</v>
+        <v>194358</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="4">
-        <v>38169</v>
+        <v>44013</v>
       </c>
       <c r="B6" s="2">
-        <v>141348</v>
+        <v>215166</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="4">
-        <v>38534</v>
-      </c>
-      <c r="B7" s="2">
-        <v>149153</v>
+        <v>45839</v>
+      </c>
+      <c r="C7" s="2">
+        <v>248441</v>
+      </c>
+      <c r="D7" s="2">
+        <v>238464</v>
+      </c>
+      <c r="E7" s="2">
+        <v>247016</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="4">
-        <v>38899</v>
-      </c>
-      <c r="B8" s="2">
-        <v>156164</v>
+        <v>47665</v>
+      </c>
+      <c r="C8" s="2">
+        <v>287218</v>
+      </c>
+      <c r="D8" s="2">
+        <v>256467</v>
+      </c>
+      <c r="E8" s="2">
+        <v>277484</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="4">
-        <v>39264</v>
-      </c>
-      <c r="B9" s="2">
-        <v>161796</v>
+        <v>49491</v>
+      </c>
+      <c r="C9" s="2">
+        <v>329249</v>
+      </c>
+      <c r="D9" s="2">
+        <v>271216</v>
+      </c>
+      <c r="E9" s="2">
+        <v>310863</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="4">
-        <v>39630</v>
-      </c>
-      <c r="B10" s="2">
-        <v>166652</v>
+        <v>51318</v>
+      </c>
+      <c r="C10" s="2">
+        <v>373888</v>
+      </c>
+      <c r="D10" s="2">
+        <v>283357</v>
+      </c>
+      <c r="E10" s="2">
+        <v>340917</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="4">
-        <v>39995</v>
-      </c>
-      <c r="B11" s="2">
-        <v>170676</v>
+        <v>53144</v>
+      </c>
+      <c r="C11" s="2">
+        <v>420768</v>
+      </c>
+      <c r="D11" s="2">
+        <v>293257</v>
+      </c>
+      <c r="E11" s="2">
+        <v>369307</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="4">
-        <v>40360</v>
-      </c>
-      <c r="B12" s="2">
-        <v>175149</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="4">
-        <v>40725</v>
-      </c>
-      <c r="B13" s="2">
-        <v>178759</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="4">
-        <v>41091</v>
-      </c>
-      <c r="B14" s="2">
-        <v>181549</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="4">
-        <v>41456</v>
-      </c>
-      <c r="B15" s="2">
-        <v>186000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="4">
-        <v>41821</v>
-      </c>
-      <c r="B16" s="2">
-        <v>190243</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="4">
-        <v>42186</v>
-      </c>
-      <c r="B17" s="2">
-        <v>194358</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="4">
-        <v>42552</v>
-      </c>
-      <c r="B18" s="2">
-        <v>198317</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="4">
-        <v>42917</v>
-      </c>
-      <c r="B19" s="2">
-        <v>202171</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="4">
-        <v>43282</v>
-      </c>
-      <c r="B20" s="2">
-        <v>206501</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="4">
-        <v>43647</v>
-      </c>
-      <c r="B21" s="2">
-        <v>211062</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="4">
-        <v>44013</v>
-      </c>
-      <c r="B22" s="2">
-        <v>215166</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="4">
-        <v>44378</v>
-      </c>
-      <c r="B23" s="2">
-        <v>221282</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="4">
-        <v>44743</v>
-      </c>
-      <c r="B24" s="2">
-        <v>226526</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="4">
-        <v>45108</v>
-      </c>
-      <c r="B25" s="2">
-        <v>231636</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="4">
-        <v>45292</v>
-      </c>
-      <c r="B26" s="2">
-        <v>234305</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="4">
-        <v>45839</v>
-      </c>
-      <c r="C27" s="2">
-        <v>248441</v>
-      </c>
-      <c r="D27" s="2">
-        <v>238464</v>
-      </c>
-      <c r="E27" s="2">
-        <v>247016</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="4">
-        <v>47665</v>
-      </c>
-      <c r="C28" s="2">
-        <v>287218</v>
-      </c>
-      <c r="D28" s="2">
-        <v>256467</v>
-      </c>
-      <c r="E28" s="2">
-        <v>277484</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="4">
-        <v>49491</v>
-      </c>
-      <c r="C29" s="2">
-        <v>329249</v>
-      </c>
-      <c r="D29" s="2">
-        <v>271216</v>
-      </c>
-      <c r="E29" s="2">
-        <v>310863</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="4">
-        <v>51318</v>
-      </c>
-      <c r="C30" s="2">
-        <v>373888</v>
-      </c>
-      <c r="D30" s="2">
-        <v>283357</v>
-      </c>
-      <c r="E30" s="2">
-        <v>340917</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="4">
-        <v>53144</v>
-      </c>
-      <c r="C31" s="2">
-        <v>420768</v>
-      </c>
-      <c r="D31" s="2">
-        <v>293257</v>
-      </c>
-      <c r="E31" s="2">
-        <v>369307</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="4">
         <v>54970</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C12" s="2">
         <v>469644</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D12" s="2">
         <v>301161</v>
       </c>
-      <c r="E32" s="2">
+      <c r="E12" s="2">
         <v>397697</v>
       </c>
     </row>

</xml_diff>